<commit_message>
Added files for demo poresentation
</commit_message>
<xml_diff>
--- a/SchoolSubjectList/PA_PRIMAVERA.pdf.xlsx
+++ b/SchoolSubjectList/PA_PRIMAVERA.pdf.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,27 +424,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>60883</t>
+          <t>49971</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Recuperacion de la Informacion</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>GUERRERO - TORRES VICTOR</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2059</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -461,27 +461,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>60883</t>
+          <t>49971</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Recuperacion de la Informacion</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GUERRERO - TORRES VICTOR</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1900</t>
+          <t>0900</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2059</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -498,27 +498,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>60883</t>
+          <t>49971</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Recuperacion de la Informacion</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GUERRERO - TORRES VICTOR</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1900</t>
+          <t>0900</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2059</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -528,229 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1CCO4/103</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>41883</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Sistemas Operativos I</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>GONZALEZ - FLORES MARCOS</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1359</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1CCO1/003</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>41883</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sistemas Operativos I</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GONZALEZ - FLORES MARCOS</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1459</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1CCO1/003</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>41883</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Sistemas Operativos I</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GONZALEZ - FLORES MARCOS</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1459</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1CCO3/109</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>42437</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Web Semantica</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>TOVAR - VIDAL MIREYA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0900</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0959</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1CCO4/104</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>42437</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Web Semantica</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>TOVAR - VIDAL MIREYA</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0900</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1059</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1CCO4/104</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>42437</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Web Semantica</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>TOVAR - VIDAL MIREYA</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0900</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1059</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1CCO3/114</t>
+          <t>1CCO4/308</t>
         </is>
       </c>
     </row>

</xml_diff>